<commit_message>
handle form submission and form retrieval from the app instead of ONA
</commit_message>
<xml_diff>
--- a/backend/xlsForms/other_activities.xlsx
+++ b/backend/xlsForms/other_activities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -472,8 +472,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,8 +1215,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="1" sqref="2:4 L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>